<commit_message>
finalize code and outputs
</commit_message>
<xml_diff>
--- a/data processing/goFlux_reprocessing/results/CH4_best_all.xlsx
+++ b/data processing/goFlux_reprocessing/results/CH4_best_all.xlsx
@@ -1460,7 +1460,7 @@
         <v>53</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.00544185948461986</v>
+        <v>-0.00266485498943696</v>
       </c>
       <c r="C5" t="n">
         <v>1966.79506874272</v>
@@ -1481,10 +1481,10 @@
         <v>1333.75046647897</v>
       </c>
       <c r="I5" t="n">
-        <v>0.00501377004647875</v>
+        <v>0.00245522293352595</v>
       </c>
       <c r="J5" t="n">
-        <v>-92.133397796268</v>
+        <v>-92.1334535371733</v>
       </c>
       <c r="K5" t="n">
         <v>0.000714570624363642</v>
@@ -1493,7 +1493,7 @@
         <v>0.278806173790103</v>
       </c>
       <c r="M5" t="n">
-        <v>-0.00721538338510404</v>
+        <v>-0.00353334195211</v>
       </c>
       <c r="N5" t="n">
         <v>1966.83631735011</v>
@@ -1514,10 +1514,10 @@
         <v>1335.80816555211</v>
       </c>
       <c r="T5" t="n">
-        <v>0.0245549447262063</v>
+        <v>0.0120244572176948</v>
       </c>
       <c r="U5" t="n">
-        <v>-340.313790905405</v>
+        <v>-340.313996795986</v>
       </c>
       <c r="V5" t="n">
         <v>0.000746568260286185</v>
@@ -1532,13 +1532,13 @@
         <v>1966.07</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.00929990795041514</v>
+        <v>0.00455412459160537</v>
       </c>
       <c r="AA5" t="n">
         <v>1.4</v>
       </c>
       <c r="AB5" t="n">
-        <v>1.64741226550211</v>
+        <v>0.806730641941524</v>
       </c>
       <c r="AC5" t="n">
         <v>250</v>
@@ -1559,7 +1559,7 @@
         <v>55</v>
       </c>
       <c r="AI5" t="n">
-        <v>-0.00721538338510404</v>
+        <v>-0.00353334195211</v>
       </c>
       <c r="AJ5" t="s">
         <v>50</v>
@@ -1583,7 +1583,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ5" t="n">
-        <v>0.0093</v>
+        <v>0.0046</v>
       </c>
     </row>
     <row r="6">
@@ -1591,7 +1591,7 @@
         <v>57</v>
       </c>
       <c r="B6" t="n">
-        <v>0.00682263829944156</v>
+        <v>0.00334101638691257</v>
       </c>
       <c r="C6" t="n">
         <v>1964.27684003335</v>
@@ -1612,10 +1612,10 @@
         <v>875.495415275172</v>
       </c>
       <c r="I6" t="n">
-        <v>0.00646311056182483</v>
+        <v>0.00316495834749785</v>
       </c>
       <c r="J6" t="n">
-        <v>94.7303708354851</v>
+        <v>94.7304047922548</v>
       </c>
       <c r="K6" t="n">
         <v>0.000638417369216882</v>
@@ -1641,13 +1641,13 @@
         <v>1965.13</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.0128421299051504</v>
+        <v>0.00628873532097979</v>
       </c>
       <c r="AA6" t="n">
         <v>1.4</v>
       </c>
       <c r="AB6" t="n">
-        <v>1.64195803787281</v>
+        <v>0.804059730325273</v>
       </c>
       <c r="AC6" t="n">
         <v>180</v>
@@ -1666,7 +1666,7 @@
         <v>55</v>
       </c>
       <c r="AI6" t="n">
-        <v>0.00682263829944156</v>
+        <v>0.00334101638691257</v>
       </c>
       <c r="AJ6" t="s">
         <v>46</v>
@@ -1686,7 +1686,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ6" t="n">
-        <v>0.013</v>
+        <v>0.0063</v>
       </c>
     </row>
     <row r="7">
@@ -1956,7 +1956,7 @@
         <v>62</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.00197097421625937</v>
+        <v>-0.000965177526008335</v>
       </c>
       <c r="C9" t="n">
         <v>1967.85312519324</v>
@@ -1977,10 +1977,10 @@
         <v>1189.81058417074</v>
       </c>
       <c r="I9" t="n">
-        <v>0.00692304035901861</v>
+        <v>0.00339018415322103</v>
       </c>
       <c r="J9" t="n">
-        <v>-351.249666378567</v>
+        <v>-351.249802431864</v>
       </c>
       <c r="K9" t="n">
         <v>-0.00431266486270832</v>
@@ -1989,7 +1989,7 @@
         <v>0.776152289421202</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.00197168061933799</v>
+        <v>-0.000965523448532416</v>
       </c>
       <c r="N9" t="n">
         <v>1967.85309524445</v>
@@ -2010,10 +2010,10 @@
         <v>1191.88739650601</v>
       </c>
       <c r="T9" t="n">
-        <v>0.0268228093257276</v>
+        <v>0.013135018489243</v>
       </c>
       <c r="U9" t="n">
-        <v>-1360.40335654025</v>
+        <v>-1360.40388342801</v>
       </c>
       <c r="V9" t="n">
         <v>-0.00431303955160245</v>
@@ -2028,13 +2028,13 @@
         <v>1965.1</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.0107713183589119</v>
+        <v>0.00527466788745383</v>
       </c>
       <c r="AA9" t="n">
         <v>1.4</v>
       </c>
       <c r="AB9" t="n">
-        <v>1.64647294914797</v>
+        <v>0.806270662796514</v>
       </c>
       <c r="AC9" t="n">
         <v>215</v>
@@ -2055,7 +2055,7 @@
         <v>55</v>
       </c>
       <c r="AI9" t="n">
-        <v>-0.00197168061933799</v>
+        <v>-0.000965523448532416</v>
       </c>
       <c r="AJ9" t="s">
         <v>50</v>
@@ -2079,7 +2079,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ9" t="n">
-        <v>0.011</v>
+        <v>0.0053</v>
       </c>
     </row>
     <row r="10">
@@ -2087,7 +2087,7 @@
         <v>63</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.0040333753383525</v>
+        <v>-0.00197512641130451</v>
       </c>
       <c r="C10" t="n">
         <v>1959.48478975147</v>
@@ -2108,10 +2108,10 @@
         <v>1174.81938744492</v>
       </c>
       <c r="I10" t="n">
-        <v>0.00751296015289439</v>
+        <v>0.00367906532837549</v>
       </c>
       <c r="J10" t="n">
-        <v>-186.269799427176</v>
+        <v>-186.269866440882</v>
       </c>
       <c r="K10" t="n">
         <v>-0.00343379843307812</v>
@@ -2120,7 +2120,7 @@
         <v>0.591943829970496</v>
       </c>
       <c r="M10" t="n">
-        <v>-0.00405275247132986</v>
+        <v>-0.00198461530928905</v>
       </c>
       <c r="N10" t="n">
         <v>1959.48515153822</v>
@@ -2141,10 +2141,10 @@
         <v>1176.89852470093</v>
       </c>
       <c r="T10" t="n">
-        <v>0.0301547615326031</v>
+        <v>0.0147666612603207</v>
       </c>
       <c r="U10" t="n">
-        <v>-744.056335686058</v>
+        <v>-744.056603373204</v>
       </c>
       <c r="V10" t="n">
         <v>-0.00343443123213882</v>
@@ -2159,13 +2159,13 @@
         <v>1960.39</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.0110968254464018</v>
+        <v>0.00543406729654295</v>
       </c>
       <c r="AA10" t="n">
         <v>1.4</v>
       </c>
       <c r="AB10" t="n">
-        <v>1.64074490528941</v>
+        <v>0.803465664560279</v>
       </c>
       <c r="AC10" t="n">
         <v>209</v>
@@ -2186,7 +2186,7 @@
         <v>55</v>
       </c>
       <c r="AI10" t="n">
-        <v>-0.00405275247132986</v>
+        <v>-0.00198461530928905</v>
       </c>
       <c r="AJ10" t="s">
         <v>50</v>
@@ -2210,7 +2210,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ10" t="n">
-        <v>0.011</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="11">
@@ -2218,7 +2218,7 @@
         <v>64</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.0199555100227224</v>
+        <v>-0.0097721267153457</v>
       </c>
       <c r="C11" t="n">
         <v>1960.00588042205</v>
@@ -2239,10 +2239,10 @@
         <v>992.699066812712</v>
       </c>
       <c r="I11" t="n">
-        <v>0.00889488777419605</v>
+        <v>0.00435578830194978</v>
       </c>
       <c r="J11" t="n">
-        <v>-44.5735927774728</v>
+        <v>-44.5735961969226</v>
       </c>
       <c r="K11" t="n">
         <v>0.0220353666416618</v>
@@ -2251,7 +2251,7 @@
         <v>0.0260987151539967</v>
       </c>
       <c r="M11" t="n">
-        <v>-0.0201103349731954</v>
+        <v>-0.0098479438221496</v>
       </c>
       <c r="N11" t="n">
         <v>1960.0085975169</v>
@@ -2272,10 +2272,10 @@
         <v>994.792146838149</v>
       </c>
       <c r="T11" t="n">
-        <v>0.0355950991185614</v>
+        <v>0.0174307670071846</v>
       </c>
       <c r="U11" t="n">
-        <v>-176.999036395989</v>
+        <v>-176.999049974067</v>
       </c>
       <c r="V11" t="n">
         <v>0.0220306303821657</v>
@@ -2290,13 +2290,13 @@
         <v>1958.02</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.0127607449286764</v>
+        <v>0.00624888145094969</v>
       </c>
       <c r="AA11" t="n">
         <v>1.4</v>
       </c>
       <c r="AB11" t="n">
-        <v>1.63155238730934</v>
+        <v>0.798964128371424</v>
       </c>
       <c r="AC11" t="n">
         <v>180</v>
@@ -2317,7 +2317,7 @@
         <v>45</v>
       </c>
       <c r="AI11" t="n">
-        <v>-0.0201103349731954</v>
+        <v>-0.0098479438221496</v>
       </c>
       <c r="AJ11" t="s">
         <v>50</v>
@@ -2341,7 +2341,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ11" t="n">
-        <v>0.013</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="12">
@@ -2611,7 +2611,7 @@
         <v>67</v>
       </c>
       <c r="B14" t="n">
-        <v>0.005091225204229</v>
+        <v>0.00249315090295548</v>
       </c>
       <c r="C14" t="n">
         <v>1956.59973730689</v>
@@ -2632,10 +2632,10 @@
         <v>1078.76032223092</v>
       </c>
       <c r="I14" t="n">
-        <v>0.00687559511181512</v>
+        <v>0.00336694811091664</v>
       </c>
       <c r="J14" t="n">
-        <v>135.047946928452</v>
+        <v>135.04790692474</v>
       </c>
       <c r="K14" t="n">
         <v>-0.00225228831965074</v>
@@ -2661,13 +2661,13 @@
         <v>1953.64</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.011400004037293</v>
+        <v>0.00558253253768163</v>
       </c>
       <c r="AA14" t="n">
         <v>1.4</v>
       </c>
       <c r="AB14" t="n">
-        <v>1.63671486535421</v>
+        <v>0.801492171481435</v>
       </c>
       <c r="AC14" t="n">
         <v>202</v>
@@ -2686,7 +2686,7 @@
         <v>55</v>
       </c>
       <c r="AI14" t="n">
-        <v>0.005091225204229</v>
+        <v>0.00249315090295548</v>
       </c>
       <c r="AJ14" t="s">
         <v>46</v>
@@ -2706,7 +2706,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ14" t="n">
-        <v>0.011</v>
+        <v>0.0056</v>
       </c>
     </row>
     <row r="15">
@@ -2845,7 +2845,7 @@
         <v>69</v>
       </c>
       <c r="B16" t="n">
-        <v>0.0043791617031354</v>
+        <v>0.00214445649453715</v>
       </c>
       <c r="C16" t="n">
         <v>1955.11797165256</v>
@@ -2866,10 +2866,10 @@
         <v>1432.2008954568</v>
       </c>
       <c r="I16" t="n">
-        <v>0.00404330334120521</v>
+        <v>0.00197998964459957</v>
       </c>
       <c r="J16" t="n">
-        <v>92.3305329947116</v>
+        <v>92.3306044978508</v>
       </c>
       <c r="K16" t="n">
         <v>0.000631098192193646</v>
@@ -2895,13 +2895,13 @@
         <v>1955.54</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.00833568325999816</v>
+        <v>0.00408194794234456</v>
       </c>
       <c r="AA16" t="n">
         <v>1.4</v>
       </c>
       <c r="AB16" t="n">
-        <v>1.63141229517107</v>
+        <v>0.798895525858864</v>
       </c>
       <c r="AC16" t="n">
         <v>275</v>
@@ -2920,7 +2920,7 @@
         <v>55</v>
       </c>
       <c r="AI16" t="n">
-        <v>0.0043791617031354</v>
+        <v>0.00214445649453715</v>
       </c>
       <c r="AJ16" t="s">
         <v>46</v>
@@ -2940,7 +2940,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ16" t="n">
-        <v>0.0083</v>
+        <v>0.0041</v>
       </c>
     </row>
     <row r="17">
@@ -2948,7 +2948,7 @@
         <v>70</v>
       </c>
       <c r="B17" t="n">
-        <v>0.00114572797797389</v>
+        <v>0.0012341140509567</v>
       </c>
       <c r="C17" t="n">
         <v>1962.13922149508</v>
@@ -2969,10 +2969,10 @@
         <v>967.093904917095</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0057600892209876</v>
+        <v>0.00620444881648978</v>
       </c>
       <c r="J17" t="n">
-        <v>502.744921283475</v>
+        <v>502.745172675089</v>
       </c>
       <c r="K17" t="n">
         <v>-0.00489919278132955</v>
@@ -2998,13 +2998,13 @@
         <v>1963.05</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.0119381799057788</v>
+        <v>0.012859139209138</v>
       </c>
       <c r="AA17" t="n">
         <v>1.4</v>
       </c>
       <c r="AB17" t="n">
-        <v>1.67987245817031</v>
+        <v>1.80946458871443</v>
       </c>
       <c r="AC17" t="n">
         <v>198</v>
@@ -3023,7 +3023,7 @@
         <v>55</v>
       </c>
       <c r="AI17" t="n">
-        <v>0.00114572797797389</v>
+        <v>0.0012341140509567</v>
       </c>
       <c r="AJ17" t="s">
         <v>46</v>
@@ -3043,7 +3043,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ17" t="n">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="18">
@@ -3051,7 +3051,7 @@
         <v>71</v>
       </c>
       <c r="B18" t="n">
-        <v>-0.0134281298630519</v>
+        <v>-0.0144640299099348</v>
       </c>
       <c r="C18" t="n">
         <v>1969.94431989695</v>
@@ -3072,10 +3072,10 @@
         <v>1955.02171158734</v>
       </c>
       <c r="I18" t="n">
-        <v>0.00535409198597112</v>
+        <v>0.00576712887759226</v>
       </c>
       <c r="J18" t="n">
-        <v>-39.8722088673208</v>
+        <v>-39.8722134391539</v>
       </c>
       <c r="K18" t="n">
         <v>0.0164141654173576</v>
@@ -3084,7 +3084,7 @@
         <v>0.0126421667986303</v>
       </c>
       <c r="M18" t="n">
-        <v>-0.0345374969002727</v>
+        <v>-0.0372018585815412</v>
       </c>
       <c r="N18" t="n">
         <v>1970.61392775619</v>
@@ -3105,10 +3105,10 @@
         <v>1954.87500272693</v>
       </c>
       <c r="T18" t="n">
-        <v>0.0395448819423663</v>
+        <v>0.0425955383673582</v>
       </c>
       <c r="U18" t="n">
-        <v>-114.498401712644</v>
+        <v>-114.498414841277</v>
       </c>
       <c r="V18" t="n">
         <v>0.0231894387383275</v>
@@ -3123,13 +3123,13 @@
         <v>1967.83</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.00740987526149185</v>
+        <v>0.0079815028975856</v>
       </c>
       <c r="AA18" t="n">
         <v>1.4</v>
       </c>
       <c r="AB18" t="n">
-        <v>1.67780746992351</v>
+        <v>1.80724029895331</v>
       </c>
       <c r="AC18" t="n">
         <v>318</v>
@@ -3150,7 +3150,7 @@
         <v>45</v>
       </c>
       <c r="AI18" t="n">
-        <v>-0.0134281298630519</v>
+        <v>-0.0144640299099348</v>
       </c>
       <c r="AJ18" t="s">
         <v>46</v>
@@ -3174,7 +3174,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ18" t="n">
-        <v>0.0074</v>
+        <v>0.008</v>
       </c>
     </row>
     <row r="19">
@@ -7683,7 +7683,7 @@
         <v>110</v>
       </c>
       <c r="B54" t="n">
-        <v>0.00724737756843108</v>
+        <v>0.00780646947769043</v>
       </c>
       <c r="C54" t="n">
         <v>2078.54897234722</v>
@@ -7704,10 +7704,10 @@
         <v>26.1053377934003</v>
       </c>
       <c r="I54" t="n">
-        <v>0.00327634979033041</v>
+        <v>0.00352909991500439</v>
       </c>
       <c r="J54" t="n">
-        <v>45.2073837659831</v>
+        <v>45.207374794585</v>
       </c>
       <c r="K54" t="n">
         <v>0.186333013802759</v>
@@ -7733,13 +7733,13 @@
         <v>2079.07</v>
       </c>
       <c r="Z54" t="n">
-        <v>0.0137694688449488</v>
+        <v>0.0148317011563359</v>
       </c>
       <c r="AA54" t="n">
         <v>1.4</v>
       </c>
       <c r="AB54" t="n">
-        <v>1.67200693117235</v>
+        <v>1.80099228326936</v>
       </c>
       <c r="AC54" t="n">
         <v>18</v>
@@ -7758,7 +7758,7 @@
         <v>86</v>
       </c>
       <c r="AI54" t="n">
-        <v>0.00724737756843108</v>
+        <v>0.00780646947769043</v>
       </c>
       <c r="AJ54" t="s">
         <v>46</v>
@@ -7778,7 +7778,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ54" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="55">
@@ -7786,7 +7786,7 @@
         <v>111</v>
       </c>
       <c r="B55" t="n">
-        <v>0.010635592614721</v>
+        <v>0.00913002548279058</v>
       </c>
       <c r="C55" t="n">
         <v>2025.59350758816</v>
@@ -7807,10 +7807,10 @@
         <v>59.5677593732558</v>
       </c>
       <c r="I55" t="n">
-        <v>0.00237364051405326</v>
+        <v>0.002037629761632</v>
       </c>
       <c r="J55" t="n">
-        <v>22.3178961440084</v>
+        <v>22.3178978577089</v>
       </c>
       <c r="K55" t="n">
         <v>0.3809502067658</v>
@@ -7819,7 +7819,7 @@
         <v>0.000100479748345382</v>
       </c>
       <c r="M55" t="n">
-        <v>0.0107409617706916</v>
+        <v>0.0092204786539453</v>
       </c>
       <c r="N55" t="n">
         <v>2025.59104478062</v>
@@ -7840,10 +7840,10 @@
         <v>62.1943407417427</v>
       </c>
       <c r="T55" t="n">
-        <v>0.00946665154545593</v>
+        <v>0.00812655952652952</v>
       </c>
       <c r="U55" t="n">
-        <v>88.1359765313308</v>
+        <v>88.1359832990046</v>
       </c>
       <c r="V55" t="n">
         <v>0.380907093177421</v>
@@ -7858,13 +7858,13 @@
         <v>2027.2</v>
       </c>
       <c r="Z55" t="n">
-        <v>0.00981121522936562</v>
+        <v>0.00842234638973157</v>
       </c>
       <c r="AA55" t="n">
         <v>1.4</v>
       </c>
       <c r="AB55" t="n">
-        <v>2.16547536133856</v>
+        <v>1.8589321674479</v>
       </c>
       <c r="AC55" t="n">
         <v>32</v>
@@ -7885,7 +7885,7 @@
         <v>60</v>
       </c>
       <c r="AI55" t="n">
-        <v>0.0107409617706916</v>
+        <v>0.0092204786539453</v>
       </c>
       <c r="AJ55" t="s">
         <v>50</v>
@@ -7909,7 +7909,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ55" t="n">
-        <v>0.0098</v>
+        <v>0.0084</v>
       </c>
     </row>
     <row r="56">
@@ -8703,7 +8703,7 @@
         <v>118</v>
       </c>
       <c r="B62" t="n">
-        <v>0.0134150697815521</v>
+        <v>0.0115160417849643</v>
       </c>
       <c r="C62" t="n">
         <v>2029.69424115738</v>
@@ -8724,10 +8724,10 @@
         <v>31.9626757192142</v>
       </c>
       <c r="I62" t="n">
-        <v>0.00497468591436414</v>
+        <v>0.00427047264477973</v>
       </c>
       <c r="J62" t="n">
-        <v>37.0828180201131</v>
+        <v>37.0828165138772</v>
       </c>
       <c r="K62" t="n">
         <v>0.269508790787866</v>
@@ -8736,7 +8736,7 @@
         <v>0.0158800299602411</v>
       </c>
       <c r="M62" t="n">
-        <v>0.0194630433362203</v>
+        <v>0.0167078683877372</v>
       </c>
       <c r="N62" t="n">
         <v>2029.62082863305</v>
@@ -8757,10 +8757,10 @@
         <v>35.0127795917089</v>
       </c>
       <c r="T62" t="n">
-        <v>0.0252661745619563</v>
+        <v>0.0216895114912708</v>
       </c>
       <c r="U62" t="n">
-        <v>129.816155292305</v>
+        <v>129.816150019411</v>
       </c>
       <c r="V62" t="n">
         <v>0.282082811883527</v>
@@ -8775,13 +8775,13 @@
         <v>2030.48</v>
       </c>
       <c r="Z62" t="n">
-        <v>0.017856464060284</v>
+        <v>0.015328715362534</v>
       </c>
       <c r="AA62" t="n">
         <v>1.4</v>
       </c>
       <c r="AB62" t="n">
-        <v>2.16828492160591</v>
+        <v>1.8613440083077</v>
       </c>
       <c r="AC62" t="n">
         <v>18</v>
@@ -8802,7 +8802,7 @@
         <v>86</v>
       </c>
       <c r="AI62" t="n">
-        <v>0.0194630433362203</v>
+        <v>0.0167078683877372</v>
       </c>
       <c r="AJ62" t="s">
         <v>50</v>
@@ -8826,7 +8826,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ62" t="n">
-        <v>0.018</v>
+        <v>0.015</v>
       </c>
     </row>
     <row r="63">
@@ -10144,7 +10144,7 @@
         <v>131</v>
       </c>
       <c r="B73" t="n">
-        <v>0.0164688206184033</v>
+        <v>0.0108843619812514</v>
       </c>
       <c r="C73" t="n">
         <v>2066.59893404031</v>
@@ -10165,10 +10165,10 @@
         <v>628.713883044909</v>
       </c>
       <c r="I73" t="n">
-        <v>0.00438340784401334</v>
+        <v>0.00289702555597273</v>
       </c>
       <c r="J73" t="n">
-        <v>26.6164040861253</v>
+        <v>26.6164021461519</v>
       </c>
       <c r="K73" t="n">
         <v>0.0686268302185884</v>
@@ -10177,7 +10177,7 @@
         <v>0.000233161764926475</v>
       </c>
       <c r="M73" t="n">
-        <v>0.0183831515974036</v>
+        <v>0.0121495570920706</v>
       </c>
       <c r="N73" t="n">
         <v>2066.57376518001</v>
@@ -10198,10 +10198,10 @@
         <v>630.797534633236</v>
       </c>
       <c r="T73" t="n">
-        <v>0.0190635841520127</v>
+        <v>0.0125992589423878</v>
       </c>
       <c r="U73" t="n">
-        <v>103.701392283058</v>
+        <v>103.701384724639</v>
       </c>
       <c r="V73" t="n">
         <v>0.0686741293087725</v>
@@ -10216,13 +10216,13 @@
         <v>2069.56</v>
       </c>
       <c r="Z73" t="n">
-        <v>0.0171591390070986</v>
+        <v>0.0113405983687239</v>
       </c>
       <c r="AA73" t="n">
         <v>1.4</v>
       </c>
       <c r="AB73" t="n">
-        <v>2.18166195947397</v>
+        <v>1.44187607830919</v>
       </c>
       <c r="AC73" t="n">
         <v>179</v>
@@ -10240,10 +10240,10 @@
         <v>60</v>
       </c>
       <c r="AH73" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="AI73" t="n">
-        <v>0.0183831515974036</v>
+        <v>0.0121495570920706</v>
       </c>
       <c r="AJ73" t="s">
         <v>50</v>
@@ -10267,7 +10267,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ73" t="n">
-        <v>0.017</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="74">
@@ -10537,7 +10537,7 @@
         <v>134</v>
       </c>
       <c r="B76" t="n">
-        <v>0.0231385361036742</v>
+        <v>0.0191270102350868</v>
       </c>
       <c r="C76" t="n">
         <v>2065.2312318958</v>
@@ -10558,10 +10558,10 @@
         <v>964.58160532513</v>
       </c>
       <c r="I76" t="n">
-        <v>0.00296874952911413</v>
+        <v>0.00245405737777704</v>
       </c>
       <c r="J76" t="n">
-        <v>12.8303256343115</v>
+        <v>12.8303239639371</v>
       </c>
       <c r="K76" t="n">
         <v>0.190430495508344</v>
@@ -10570,7 +10570,7 @@
         <v>0.000000000000168686717812083</v>
       </c>
       <c r="M76" t="n">
-        <v>0.0552140397124166</v>
+        <v>0.0456415867437777</v>
       </c>
       <c r="N76" t="n">
         <v>2064.71978492108</v>
@@ -10591,10 +10591,10 @@
         <v>962.560307168814</v>
       </c>
       <c r="T76" t="n">
-        <v>0.0226121268324787</v>
+        <v>0.0186918620571649</v>
       </c>
       <c r="U76" t="n">
-        <v>40.9535816438254</v>
+        <v>40.9535763120969</v>
       </c>
       <c r="V76" t="n">
         <v>0.203298281441208</v>
@@ -10609,13 +10609,13 @@
         <v>2066.53</v>
       </c>
       <c r="Z76" t="n">
-        <v>0.0120803265785237</v>
+        <v>0.00998596147462948</v>
       </c>
       <c r="AA76" t="n">
         <v>1.4</v>
       </c>
       <c r="AB76" t="n">
-        <v>2.18308758883322</v>
+        <v>1.80460589505804</v>
       </c>
       <c r="AC76" t="n">
         <v>255</v>
@@ -10636,7 +10636,7 @@
         <v>60</v>
       </c>
       <c r="AI76" t="n">
-        <v>0.0231385361036742</v>
+        <v>0.0191270102350868</v>
       </c>
       <c r="AJ76" t="s">
         <v>46</v>
@@ -10660,7 +10660,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ76" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="77">
@@ -11978,7 +11978,7 @@
         <v>145</v>
       </c>
       <c r="B87" t="n">
-        <v>0.0212229171632795</v>
+        <v>0.0188685758094741</v>
       </c>
       <c r="C87" t="n">
         <v>2065.96076027339</v>
@@ -11999,10 +11999,10 @@
         <v>880.375693714847</v>
       </c>
       <c r="I87" t="n">
-        <v>0.00287445044968125</v>
+        <v>0.00255557711648549</v>
       </c>
       <c r="J87" t="n">
-        <v>13.5440874012113</v>
+        <v>13.5440912037586</v>
       </c>
       <c r="K87" t="n">
         <v>0.179867907991011</v>
@@ -12011,7 +12011,7 @@
         <v>0.00000000000245357828991164</v>
       </c>
       <c r="M87" t="n">
-        <v>0.0419940534760873</v>
+        <v>0.0373354885883284</v>
       </c>
       <c r="N87" t="n">
         <v>2065.62732902344</v>
@@ -12032,10 +12032,10 @@
         <v>880.046442286522</v>
       </c>
       <c r="T87" t="n">
-        <v>0.0190178104490916</v>
+        <v>0.0169080949698564</v>
       </c>
       <c r="U87" t="n">
-        <v>45.286912967144</v>
+        <v>45.2869256815943</v>
       </c>
       <c r="V87" t="n">
         <v>0.187850477721928</v>
@@ -12050,13 +12050,13 @@
         <v>2068.54</v>
       </c>
       <c r="Z87" t="n">
-        <v>0.0125461921527185</v>
+        <v>0.0111543939003537</v>
       </c>
       <c r="AA87" t="n">
         <v>1.4</v>
       </c>
       <c r="AB87" t="n">
-        <v>2.18662206090237</v>
+        <v>1.94405150834737</v>
       </c>
       <c r="AC87" t="n">
         <v>245</v>
@@ -12077,7 +12077,7 @@
         <v>60</v>
       </c>
       <c r="AI87" t="n">
-        <v>0.0419940534760873</v>
+        <v>0.0373354885883284</v>
       </c>
       <c r="AJ87" t="s">
         <v>50</v>
@@ -12101,7 +12101,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ87" t="n">
-        <v>0.013</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="88">
@@ -13681,7 +13681,7 @@
         <v>158</v>
       </c>
       <c r="B100" t="n">
-        <v>-0.0176854435225526</v>
+        <v>-0.0126140105958497</v>
       </c>
       <c r="C100" t="n">
         <v>2061.64713683895</v>
@@ -13702,10 +13702,10 @@
         <v>886.918522596414</v>
       </c>
       <c r="I100" t="n">
-        <v>0.00260530915061084</v>
+        <v>0.00185821798150038</v>
       </c>
       <c r="J100" t="n">
-        <v>-14.7313758192637</v>
+        <v>-14.7313811684269</v>
       </c>
       <c r="K100" t="n">
         <v>0.162111844285512</v>
@@ -13714,7 +13714,7 @@
         <v>0.0000000000939865707376718</v>
       </c>
       <c r="M100" t="n">
-        <v>-0.0176792761632673</v>
+        <v>-0.01260961177287</v>
       </c>
       <c r="N100" t="n">
         <v>2061.64708145017</v>
@@ -13735,10 +13735,10 @@
         <v>889.005794856872</v>
       </c>
       <c r="T100" t="n">
-        <v>0.0102810154758739</v>
+        <v>0.00733286021725542</v>
       </c>
       <c r="U100" t="n">
-        <v>-58.1529208601599</v>
+        <v>-58.1529419726648</v>
       </c>
       <c r="V100" t="n">
         <v>0.162051859678442</v>
@@ -13753,13 +13753,13 @@
         <v>2059.04</v>
       </c>
       <c r="Z100" t="n">
-        <v>0.0100773647578124</v>
+        <v>0.00718760520035526</v>
       </c>
       <c r="AA100" t="n">
         <v>1.4</v>
       </c>
       <c r="AB100" t="n">
-        <v>1.67716142040735</v>
+        <v>1.1962228654877</v>
       </c>
       <c r="AC100" t="n">
         <v>234</v>
@@ -13771,7 +13771,7 @@
         <v>1</v>
       </c>
       <c r="AF100" t="n">
-        <v>0.999651274830771</v>
+        <v>0.99965127483077</v>
       </c>
       <c r="AG100" t="s">
         <v>60</v>
@@ -13780,7 +13780,7 @@
         <v>60</v>
       </c>
       <c r="AI100" t="n">
-        <v>-0.0176792761632673</v>
+        <v>-0.01260961177287</v>
       </c>
       <c r="AJ100" t="s">
         <v>50</v>
@@ -13804,7 +13804,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ100" t="n">
-        <v>0.01</v>
+        <v>0.0072</v>
       </c>
     </row>
     <row r="101">
@@ -14074,7 +14074,7 @@
         <v>161</v>
       </c>
       <c r="B103" t="n">
-        <v>0.0153571907345666</v>
+        <v>0.00986434372811507</v>
       </c>
       <c r="C103" t="n">
         <v>2063.76355635815</v>
@@ -14095,10 +14095,10 @@
         <v>1138.24268999712</v>
       </c>
       <c r="I103" t="n">
-        <v>0.00185260974294219</v>
+        <v>0.00118998234567112</v>
       </c>
       <c r="J103" t="n">
-        <v>12.0634676938163</v>
+        <v>12.0634720207435</v>
       </c>
       <c r="K103" t="n">
         <v>0.173756537153652</v>
@@ -14107,7 +14107,7 @@
         <v>0.00000000000000314887570380767</v>
       </c>
       <c r="M103" t="n">
-        <v>0.0153684776488147</v>
+        <v>0.00987159362190732</v>
       </c>
       <c r="N103" t="n">
         <v>2063.76320158836</v>
@@ -14128,10 +14128,10 @@
         <v>1140.31540748238</v>
       </c>
       <c r="T103" t="n">
-        <v>0.00740767528493959</v>
+        <v>0.00475815419038505</v>
       </c>
       <c r="U103" t="n">
-        <v>48.2004493497176</v>
+        <v>48.2004666381892</v>
       </c>
       <c r="V103" t="n">
         <v>0.17370044137695</v>
@@ -14146,13 +14146,13 @@
         <v>2069.74</v>
       </c>
       <c r="Z103" t="n">
-        <v>0.00961718086637544</v>
+        <v>0.00617737836307835</v>
       </c>
       <c r="AA103" t="n">
         <v>1.4</v>
       </c>
       <c r="AB103" t="n">
-        <v>2.2050821843618</v>
+        <v>1.41638461039153</v>
       </c>
       <c r="AC103" t="n">
         <v>323</v>
@@ -14173,7 +14173,7 @@
         <v>60</v>
       </c>
       <c r="AI103" t="n">
-        <v>0.0153684776488147</v>
+        <v>0.00987159362190732</v>
       </c>
       <c r="AJ103" t="s">
         <v>50</v>
@@ -14197,7 +14197,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ103" t="n">
-        <v>0.0096</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="104">
@@ -14860,7 +14860,7 @@
         <v>167</v>
       </c>
       <c r="B109" t="n">
-        <v>0.0105484570010873</v>
+        <v>0.008255732675543</v>
       </c>
       <c r="C109" t="n">
         <v>2066.3763220395</v>
@@ -14881,10 +14881,10 @@
         <v>817.047483572034</v>
       </c>
       <c r="I109" t="n">
-        <v>0.00396519396451928</v>
+        <v>0.0031033527915448</v>
       </c>
       <c r="J109" t="n">
-        <v>37.5902747113684</v>
+        <v>37.5902771263204</v>
       </c>
       <c r="K109" t="n">
         <v>0.027739098313031</v>
@@ -14893,7 +14893,7 @@
         <v>0.00840497732147472</v>
       </c>
       <c r="M109" t="n">
-        <v>0.0154056838833487</v>
+        <v>0.0120572333765724</v>
       </c>
       <c r="N109" t="n">
         <v>2066.29373629679</v>
@@ -14914,10 +14914,10 @@
         <v>818.623135051865</v>
       </c>
       <c r="T109" t="n">
-        <v>0.0205634410310041</v>
+        <v>0.0160939446338208</v>
       </c>
       <c r="U109" t="n">
-        <v>133.479572777877</v>
+        <v>133.479581353147</v>
       </c>
       <c r="V109" t="n">
         <v>0.0300146582274552</v>
@@ -14932,13 +14932,13 @@
         <v>2069.82</v>
       </c>
       <c r="Z109" t="n">
-        <v>0.0144884735102521</v>
+        <v>0.0113393801733276</v>
       </c>
       <c r="AA109" t="n">
         <v>1.4</v>
       </c>
       <c r="AB109" t="n">
-        <v>2.20431775548836</v>
+        <v>1.72520569779912</v>
       </c>
       <c r="AC109" t="n">
         <v>214</v>
@@ -14959,7 +14959,7 @@
         <v>86</v>
       </c>
       <c r="AI109" t="n">
-        <v>0.0154056838833487</v>
+        <v>0.0120572333765724</v>
       </c>
       <c r="AJ109" t="s">
         <v>50</v>
@@ -14983,7 +14983,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ109" t="n">
-        <v>0.014</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="110">
@@ -16956,7 +16956,7 @@
         <v>183</v>
       </c>
       <c r="B125" t="n">
-        <v>0.0070164292496825</v>
+        <v>0.00934573959311432</v>
       </c>
       <c r="C125" t="n">
         <v>2069.94998776567</v>
@@ -16977,10 +16977,10 @@
         <v>949.001140753874</v>
       </c>
       <c r="I125" t="n">
-        <v>0.00389998420250438</v>
+        <v>0.00519469919491083</v>
       </c>
       <c r="J125" t="n">
-        <v>55.5836033361394</v>
+        <v>55.583607302071</v>
       </c>
       <c r="K125" t="n">
         <v>0.00950842282687769</v>
@@ -17006,13 +17006,13 @@
         <v>2071.76</v>
       </c>
       <c r="Z125" t="n">
-        <v>0.0132322245794477</v>
+        <v>0.0176250512556256</v>
       </c>
       <c r="AA125" t="n">
         <v>1.4</v>
       </c>
       <c r="AB125" t="n">
-        <v>2.20222023357952</v>
+        <v>2.93331210182912</v>
       </c>
       <c r="AC125" t="n">
         <v>234</v>
@@ -17031,7 +17031,7 @@
         <v>86</v>
       </c>
       <c r="AI125" t="n">
-        <v>0.0070164292496825</v>
+        <v>0.00934573959311432</v>
       </c>
       <c r="AJ125" t="s">
         <v>46</v>
@@ -17051,7 +17051,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ125" t="n">
-        <v>0.013</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="126">
@@ -17190,7 +17190,7 @@
         <v>185</v>
       </c>
       <c r="B127" t="n">
-        <v>0.00534905901263441</v>
+        <v>0.0077635109036784</v>
       </c>
       <c r="C127" t="n">
         <v>2073.54636928564</v>
@@ -17211,10 +17211,10 @@
         <v>538.579298854796</v>
       </c>
       <c r="I127" t="n">
-        <v>0.0051026988922287</v>
+        <v>0.00740594865520072</v>
       </c>
       <c r="J127" t="n">
-        <v>95.3943278654467</v>
+        <v>95.3943228403497</v>
       </c>
       <c r="K127" t="n">
         <v>0.000686279143143786</v>
@@ -17240,13 +17240,13 @@
         <v>2074.24</v>
       </c>
       <c r="Z127" t="n">
-        <v>0.0162415042925493</v>
+        <v>0.0235725751706086</v>
       </c>
       <c r="AA127" t="n">
         <v>1.4</v>
       </c>
       <c r="AB127" t="n">
-        <v>1.67055472723365</v>
+        <v>2.42460773183403</v>
       </c>
       <c r="AC127" t="n">
         <v>145</v>
@@ -17265,7 +17265,7 @@
         <v>86</v>
       </c>
       <c r="AI127" t="n">
-        <v>0.00534905901263441</v>
+        <v>0.0077635109036784</v>
       </c>
       <c r="AJ127" t="s">
         <v>46</v>
@@ -17285,7 +17285,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ127" t="n">
-        <v>0.016</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="128">
@@ -17817,7 +17817,7 @@
         <v>190</v>
       </c>
       <c r="B132" t="n">
-        <v>0.0000903842660074929</v>
+        <v>0.000180167972107959</v>
       </c>
       <c r="C132" t="n">
         <v>2079.07110111462</v>
@@ -17838,10 +17838,10 @@
         <v>654.256443595832</v>
       </c>
       <c r="I132" t="n">
-        <v>0.00288056249586597</v>
+        <v>0.00574198469755894</v>
       </c>
       <c r="J132" t="n">
-        <v>3187.01763382929</v>
+        <v>3187.01744287729</v>
       </c>
       <c r="K132" t="n">
         <v>-0.00525794888682607</v>
@@ -17867,13 +17867,13 @@
         <v>2079.2</v>
       </c>
       <c r="Z132" t="n">
-        <v>0.0122336172561616</v>
+        <v>0.0243859480189268</v>
       </c>
       <c r="AA132" t="n">
         <v>1.4</v>
       </c>
       <c r="AB132" t="n">
-        <v>1.66901492566205</v>
+        <v>3.32694005115358</v>
       </c>
       <c r="AC132" t="n">
         <v>192</v>
@@ -17892,7 +17892,7 @@
         <v>86</v>
       </c>
       <c r="AI132" t="n">
-        <v>0.0000903842660074929</v>
+        <v>0.000180167972107959</v>
       </c>
       <c r="AJ132" t="s">
         <v>46</v>
@@ -17912,7 +17912,7 @@
         <v>0.5</v>
       </c>
       <c r="AQ132" t="n">
-        <v>0.012</v>
+        <v>0.024</v>
       </c>
     </row>
     <row r="133">

</xml_diff>